<commit_message>
datas e suspenso ok
</commit_message>
<xml_diff>
--- a/ESTORNOATUALIZADA.xlsx
+++ b/ESTORNOATUALIZADA.xlsx
@@ -24,7 +24,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
@@ -34,12 +34,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -47,14 +41,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,177 +499,158 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>24/01/2024</t>
         </is>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="0" t="n">
         <v>11913013022</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="0" t="n">
         <v>1461262</v>
       </c>
-      <c r="D4" s="1" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>ESTORNO REFERENTE 07/2024 P1</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t>PLANO CLARO INTERNET MAIS 120GB</t>
         </is>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>202409</v>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>INAD_60_OK</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
+      <c r="F4" s="0" t="n">
+        <v>202409</v>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>INAD_60_OK</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>TAYNARA SANTOS DA SILVA</t>
         </is>
       </c>
-      <c r="K4" s="1" t="inlineStr">
+      <c r="K4" s="0" t="inlineStr">
         <is>
           <t>118 S BERNARDO DO CAMPO GOLDEN</t>
         </is>
       </c>
-      <c r="L4" s="2" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Suspenso</t>
         </is>
       </c>
-      <c r="M4" s="2" t="n"/>
-      <c r="N4" s="2" t="n"/>
-      <c r="O4" s="1" t="inlineStr">
+      <c r="O4" s="0" t="inlineStr">
         <is>
           <t>Pedro</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>18/03/2024</t>
         </is>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="0" t="n">
         <v>11913273279</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="0" t="n">
         <v>1535334</v>
       </c>
-      <c r="D5" s="1" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>ESTORNO REFERENTE 07/2024 P2</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>PLANO CONTROLE ON 25GB GAMING - CF</t>
         </is>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>202409</v>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>INAD_60_OK</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n"/>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
+      <c r="F5" s="0" t="n">
+        <v>202409</v>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>INAD_60_OK</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
         <is>
           <t>VANESSA FEITOSA DE ARAUJO</t>
         </is>
       </c>
-      <c r="K5" s="1" t="inlineStr">
+      <c r="K5" s="0" t="inlineStr">
         <is>
           <t>189 CAMPO LIMPO</t>
         </is>
       </c>
-      <c r="L5" s="2" t="inlineStr">
-        <is>
-          <t>Suspenso</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="n"/>
-      <c r="N5" s="2" t="n"/>
-      <c r="O5" s="1" t="inlineStr">
+      <c r="O5" s="0" t="inlineStr">
         <is>
           <t>Pedro</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>15/03/2024</t>
         </is>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="0" t="n">
         <v>11913428672</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="0" t="n">
         <v>1531787</v>
       </c>
-      <c r="D6" s="1" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>ESTORNO REFERENTE 07/2024 P2</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="E6" s="0" t="inlineStr">
         <is>
           <t>PLANO CONTROLE ON 20GB - SF</t>
         </is>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>202409</v>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>INAD_60_OK</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n"/>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
+      <c r="F6" s="0" t="n">
+        <v>202409</v>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>INAD_60_OK</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
         <is>
           <t>LETICIA APARECIDA SOARES</t>
         </is>
       </c>
-      <c r="K6" s="1" t="inlineStr">
+      <c r="K6" s="0" t="inlineStr">
         <is>
           <t>117 OSASCO SHOPPING CONTINENTAL</t>
         </is>
       </c>
-      <c r="L6" s="2" t="inlineStr">
-        <is>
-          <t>Suspenso</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="n"/>
-      <c r="N6" s="2" t="n"/>
-      <c r="O6" s="1" t="inlineStr">
+      <c r="O6" s="0" t="inlineStr">
         <is>
           <t>Pedro</t>
         </is>

</xml_diff>